<commit_message>
Fixes for Non-HMIS clients with no assessments
</commit_message>
<xml_diff>
--- a/spec/fixtures/deidentified_client_xlsxs/initial.xlsx
+++ b/spec/fixtures/deidentified_client_xlsxs/initial.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliot/Sites/boston-cas/spec/fixtures/deidentified_client_xlsxs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09239C64-6BBB-4E47-9F40-65011538C83B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5101A7B0-A138-8C42-A19C-140D22E40EEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8500" yWindow="2440" windowWidth="28040" windowHeight="17440" xr2:uid="{C75E722D-C520-B444-8D1D-2BF65DAD71B8}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
   <si>
     <t>Date Information Collected</t>
   </si>
@@ -457,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA451A2-3A3B-C841-80E6-AE79DA8D5FC0}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -583,6 +583,65 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>43840</v>
+      </c>
+      <c r="B3" s="1">
+        <v>43840</v>
+      </c>
+      <c r="C3" s="1">
+        <v>43840</v>
+      </c>
+      <c r="D3" s="3">
+        <v>24212</v>
+      </c>
+      <c r="E3" s="2">
+        <v>43840</v>
+      </c>
+      <c r="F3" s="3">
+        <v>3</v>
+      </c>
+      <c r="G3" s="3">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="2">
+        <v>36170</v>
+      </c>
+      <c r="J3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>17</v>
+      </c>
+      <c r="R3" s="2">
+        <v>43840</v>
+      </c>
+      <c r="S3">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Removing extra line from test file
</commit_message>
<xml_diff>
--- a/spec/fixtures/deidentified_client_xlsxs/initial.xlsx
+++ b/spec/fixtures/deidentified_client_xlsxs/initial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliot/Sites/boston-cas/spec/fixtures/deidentified_client_xlsxs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5101A7B0-A138-8C42-A19C-140D22E40EEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8884062D-CE3A-464F-A5A1-228C2F44E068}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8500" yWindow="2440" windowWidth="28040" windowHeight="17440" xr2:uid="{C75E722D-C520-B444-8D1D-2BF65DAD71B8}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Date Information Collected</t>
   </si>
@@ -457,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA451A2-3A3B-C841-80E6-AE79DA8D5FC0}">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -583,65 +583,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>43840</v>
-      </c>
-      <c r="B3" s="1">
-        <v>43840</v>
-      </c>
-      <c r="C3" s="1">
-        <v>43840</v>
-      </c>
-      <c r="D3" s="3">
-        <v>24212</v>
-      </c>
-      <c r="E3" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F3" s="3">
-        <v>3</v>
-      </c>
-      <c r="G3" s="3">
-        <v>3</v>
-      </c>
-      <c r="H3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="2">
-        <v>36170</v>
-      </c>
-      <c r="J3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" t="s">
-        <v>16</v>
-      </c>
-      <c r="M3" t="s">
-        <v>17</v>
-      </c>
-      <c r="N3" t="s">
-        <v>17</v>
-      </c>
-      <c r="O3" t="s">
-        <v>17</v>
-      </c>
-      <c r="P3" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>17</v>
-      </c>
-      <c r="R3" s="2">
-        <v>43840</v>
-      </c>
-      <c r="S3">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add Health Prioritized to De-identified importer
</commit_message>
<xml_diff>
--- a/spec/fixtures/deidentified_client_xlsxs/initial.xlsx
+++ b/spec/fixtures/deidentified_client_xlsxs/initial.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliot/Sites/boston-cas/spec/fixtures/deidentified_client_xlsxs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8884062D-CE3A-464F-A5A1-228C2F44E068}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91CC435-1057-874C-95F4-7C292AC08128}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8500" yWindow="2440" windowWidth="28040" windowHeight="17440" xr2:uid="{C75E722D-C520-B444-8D1D-2BF65DAD71B8}"/>
+    <workbookView xWindow="4660" yWindow="1020" windowWidth="30880" windowHeight="17560" xr2:uid="{C75E722D-C520-B444-8D1D-2BF65DAD71B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,19 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
-  <si>
-    <t>Date Information Collected</t>
-  </si>
-  <si>
-    <t>Date Entered Program</t>
-  </si>
-  <si>
-    <t>Date Exit Program</t>
-  </si>
-  <si>
-    <t>Homebase ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Date First became Homeless</t>
   </si>
@@ -56,30 +44,9 @@
     <t>Cumulative Months Homeless in Last Three Years</t>
   </si>
   <si>
-    <t>Family of at least One Adult and Once Child</t>
-  </si>
-  <si>
-    <t>Date of Birth (Client)</t>
-  </si>
-  <si>
     <t>Veteran Status</t>
   </si>
   <si>
-    <t>Developmental Disability</t>
-  </si>
-  <si>
-    <t>Chronic Health Condition</t>
-  </si>
-  <si>
-    <t>Mental Health Problem</t>
-  </si>
-  <si>
-    <t>Substance Abuse Disorder</t>
-  </si>
-  <si>
-    <t>HOPWA</t>
-  </si>
-  <si>
     <t>VI-SPDAT Score</t>
   </si>
   <si>
@@ -89,30 +56,59 @@
     <t>No</t>
   </si>
   <si>
-    <t xml:space="preserve">Disabling Condition* </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Physical Disabilty </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Client's last residential zip code </t>
+    <t>Prioritized for Health</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Shelter Location</t>
+  </si>
+  <si>
+    <t>Referral Date</t>
+  </si>
+  <si>
+    <t>Home-base ID</t>
+  </si>
+  <si>
+    <t>Family of at least one Adult and one child</t>
+  </si>
+  <si>
+    <t>Age greater than 65 years of age</t>
+  </si>
+  <si>
+    <t>Age less than 24 years of age</t>
+  </si>
+  <si>
+    <t>Permanent Supportive Housing Eligible</t>
+  </si>
+  <si>
+    <t>Minimum Bedroom Size</t>
+  </si>
+  <si>
+    <t>HOPWA Eligible</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Inside</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -138,10 +134,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -457,130 +452,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA451A2-3A3B-C841-80E6-AE79DA8D5FC0}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="O1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" t="s">
-        <v>20</v>
-      </c>
-      <c r="S1" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>43840</v>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="B2" s="1">
         <v>43840</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
+        <v>5555</v>
+      </c>
+      <c r="D2" s="1">
         <v>43840</v>
       </c>
-      <c r="D2" s="3">
-        <v>1234</v>
-      </c>
-      <c r="E2" s="2">
-        <v>43840</v>
-      </c>
-      <c r="F2" s="3">
+      <c r="E2">
         <v>3</v>
       </c>
-      <c r="G2" s="3">
+      <c r="F2">
         <v>3</v>
       </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
       <c r="H2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="2">
-        <v>36170</v>
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
       </c>
       <c r="J2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" t="s">
-        <v>17</v>
+        <v>6</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
       </c>
       <c r="L2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="M2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="N2">
+        <v>3</v>
       </c>
       <c r="O2" t="s">
-        <v>17</v>
-      </c>
-      <c r="P2" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>17</v>
-      </c>
-      <c r="R2" s="2">
-        <v>43840</v>
-      </c>
-      <c r="S2">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Keep most recent assessment in-sync with client changes when uploading
</commit_message>
<xml_diff>
--- a/spec/fixtures/deidentified_client_xlsxs/initial.xlsx
+++ b/spec/fixtures/deidentified_client_xlsxs/initial.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliot/Sites/boston-cas/spec/fixtures/deidentified_client_xlsxs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliot/Sites/vagrant/op/boston-cas/spec/fixtures/deidentified_client_xlsxs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91CC435-1057-874C-95F4-7C292AC08128}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24839A62-E6B5-F540-9B9B-46C711DCB571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4660" yWindow="1020" windowWidth="30880" windowHeight="17560" xr2:uid="{C75E722D-C520-B444-8D1D-2BF65DAD71B8}"/>
+    <workbookView xWindow="4820" yWindow="9900" windowWidth="58620" windowHeight="21760" xr2:uid="{C75E722D-C520-B444-8D1D-2BF65DAD71B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,23 +33,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
-  <si>
-    <t>Date First became Homeless</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Occurrences of Homelessness in Last Three Years</t>
   </si>
   <si>
-    <t>Cumulative Months Homeless in Last Three Years</t>
-  </si>
-  <si>
     <t>Veteran Status</t>
   </si>
   <si>
-    <t>VI-SPDAT Score</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -59,33 +50,21 @@
     <t>Prioritized for Health</t>
   </si>
   <si>
-    <t>n</t>
-  </si>
-  <si>
     <t>Shelter Location</t>
   </si>
   <si>
-    <t>Referral Date</t>
-  </si>
-  <si>
     <t>Home-base ID</t>
   </si>
   <si>
     <t>Family of at least one Adult and one child</t>
   </si>
   <si>
-    <t>Age greater than 65 years of age</t>
-  </si>
-  <si>
     <t>Age less than 24 years of age</t>
   </si>
   <si>
     <t>Permanent Supportive Housing Eligible</t>
   </si>
   <si>
-    <t>Minimum Bedroom Size</t>
-  </si>
-  <si>
     <t>HOPWA Eligible</t>
   </si>
   <si>
@@ -99,6 +78,30 @@
   </si>
   <si>
     <t>Inside</t>
+  </si>
+  <si>
+    <t>Disabled Per HUD Language</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Substance Use Disability</t>
+  </si>
+  <si>
+    <t>Mental Health Disability</t>
+  </si>
+  <si>
+    <t>Cumulative days Homeless</t>
+  </si>
+  <si>
+    <t>Age greater than 60 years of age</t>
+  </si>
+  <si>
+    <t>Currently first time pregnant 28 weeks or less</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -134,10 +137,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -156,7 +158,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -444,7 +446,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -455,103 +457,119 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A3" sqref="A3:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="34" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="39.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>4</v>
-      </c>
-      <c r="O1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="1">
-        <v>43840</v>
-      </c>
-      <c r="C2" s="2">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2">
         <v>5555</v>
       </c>
-      <c r="D2" s="1">
-        <v>43840</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
       </c>
       <c r="F2">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
-        <v>5</v>
+      <c r="G2">
+        <v>200</v>
       </c>
       <c r="H2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="J2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2">
+        <v>3</v>
+      </c>
+      <c r="K2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" t="s">
         <v>2</v>
-      </c>
-      <c r="L2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2">
-        <v>3</v>
-      </c>
-      <c r="O2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>